<commit_message>
add 4 departments title and xls import function.
</commit_message>
<xml_diff>
--- a/Release/表一：耕保.xlsx
+++ b/Release/表一：耕保.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>报批面积</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,6 +103,50 @@
   </si>
   <si>
     <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -457,98 +501,98 @@
   </cellStyleXfs>
   <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,273 +895,303 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="5.75" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="6.25" style="2" customWidth="1"/>
-    <col min="16" max="17" width="4.5" style="2" customWidth="1"/>
-    <col min="18" max="18" width="5.125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="4.25" style="2" customWidth="1"/>
+    <col min="1" max="1" width="6" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="30" customWidth="1"/>
+    <col min="3" max="4" width="4.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.625" style="30" customWidth="1"/>
+    <col min="8" max="9" width="7.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.875" style="30" customWidth="1"/>
+    <col min="11" max="11" width="7" style="30" customWidth="1"/>
+    <col min="12" max="12" width="6.125" style="30" customWidth="1"/>
+    <col min="13" max="13" width="5.75" style="30" customWidth="1"/>
+    <col min="14" max="14" width="8.375" style="31" customWidth="1"/>
+    <col min="15" max="15" width="6.25" style="31" customWidth="1"/>
+    <col min="16" max="17" width="4.5" style="31" customWidth="1"/>
+    <col min="18" max="18" width="5.125" style="31" customWidth="1"/>
+    <col min="19" max="19" width="4.25" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="33" customHeight="1" thickBot="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:19" ht="19.5" customHeight="1">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="R2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="24" t="s">
+      <c r="S2" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="21" customHeight="1">
-      <c r="A3" s="28"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="14" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="14" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="25"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="14"/>
     </row>
     <row r="4" spans="1:19" ht="24.75" customHeight="1">
-      <c r="A4" s="29"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="3" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="26"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="19"/>
     </row>
     <row r="5" spans="1:19" ht="21" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="8"/>
+      <c r="A5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" s="24" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:19" ht="21" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="8"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="24"/>
     </row>
     <row r="7" spans="1:19" ht="21" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="8"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="24"/>
     </row>
     <row r="8" spans="1:19" ht="21" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="8"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="24"/>
     </row>
     <row r="9" spans="1:19" ht="21" customHeight="1" thickBot="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="13"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="R2:R4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="P2:P4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="K2:K4"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="L2:L4"/>
     <mergeCell ref="M2:M4"/>
@@ -1130,6 +1204,14 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="R2:R4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="K2:K4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>